<commit_message>
Feat: Banco de dados criado
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -465,7 +465,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Avaliacao</t>
+          <t>Avaliação</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -599,7 +599,9 @@
       <c r="D6" s="2" t="n">
         <v>45474</v>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
@@ -732,7 +734,9 @@
       <c r="D11" s="2" t="n">
         <v>45476</v>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>5</v>
+      </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
@@ -757,7 +761,9 @@
       <c r="D12" s="2" t="n">
         <v>45477</v>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>99</v>
+      </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
@@ -836,7 +842,9 @@
       <c r="D15" s="2" t="n">
         <v>45478</v>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
@@ -996,7 +1004,9 @@
       <c r="D21" s="2" t="n">
         <v>45487</v>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="n">
+        <v>5</v>
+      </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
@@ -1021,7 +1031,9 @@
       <c r="D22" s="2" t="n">
         <v>45487</v>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>99</v>
+      </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
@@ -1289,7 +1301,9 @@
       <c r="D32" s="2" t="n">
         <v>45491</v>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="n">
+        <v>99</v>
+      </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
@@ -1368,7 +1382,9 @@
       <c r="D35" s="2" t="n">
         <v>45492</v>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="n">
+        <v>5</v>
+      </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
@@ -1447,7 +1463,9 @@
       <c r="D38" s="2" t="n">
         <v>45499</v>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="n">
+        <v>99</v>
+      </c>
       <c r="F38" t="n">
         <v>1</v>
       </c>
@@ -1634,7 +1652,9 @@
       <c r="D45" s="2" t="n">
         <v>45502</v>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="n">
+        <v>99</v>
+      </c>
       <c r="F45" t="n">
         <v>0</v>
       </c>
@@ -1659,7 +1679,9 @@
       <c r="D46" s="2" t="n">
         <v>45502</v>
       </c>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="n">
+        <v>99</v>
+      </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
@@ -1711,7 +1733,9 @@
       <c r="D48" s="2" t="n">
         <v>45502</v>
       </c>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="n">
+        <v>5</v>
+      </c>
       <c r="F48" t="n">
         <v>0</v>
       </c>
@@ -2060,7 +2084,9 @@
       <c r="D61" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>99</v>
+      </c>
       <c r="F61" t="n">
         <v>0</v>
       </c>
@@ -2166,7 +2192,9 @@
       <c r="D65" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>99</v>
+      </c>
       <c r="F65" t="n">
         <v>0</v>
       </c>
@@ -2191,7 +2219,9 @@
       <c r="D66" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>99</v>
+      </c>
       <c r="F66" t="n">
         <v>0</v>
       </c>
@@ -2297,7 +2327,9 @@
       <c r="D70" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="E70" t="inlineStr"/>
+      <c r="E70" t="n">
+        <v>5</v>
+      </c>
       <c r="F70" t="n">
         <v>0</v>
       </c>
@@ -2322,7 +2354,9 @@
       <c r="D71" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="E71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>5</v>
+      </c>
       <c r="F71" t="n">
         <v>0</v>
       </c>
@@ -2347,7 +2381,9 @@
       <c r="D72" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>5</v>
+      </c>
       <c r="F72" t="n">
         <v>0</v>
       </c>
@@ -2372,7 +2408,9 @@
       <c r="D73" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>5</v>
+      </c>
       <c r="F73" t="n">
         <v>0</v>
       </c>
@@ -2397,7 +2435,9 @@
       <c r="D74" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>99</v>
+      </c>
       <c r="F74" t="n">
         <v>0</v>
       </c>
@@ -2617,7 +2657,9 @@
       <c r="F82" t="n">
         <v>1</v>
       </c>
-      <c r="G82" t="inlineStr"/>
+      <c r="G82" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -2771,7 +2813,9 @@
       <c r="D88" s="2" t="n">
         <v>45544</v>
       </c>
-      <c r="E88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>99</v>
+      </c>
       <c r="F88" t="n">
         <v>0</v>
       </c>
@@ -2796,7 +2840,9 @@
       <c r="D89" s="2" t="n">
         <v>45544</v>
       </c>
-      <c r="E89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>2</v>
+      </c>
       <c r="F89" t="n">
         <v>0</v>
       </c>
@@ -2821,7 +2867,9 @@
       <c r="D90" s="2" t="n">
         <v>45544</v>
       </c>
-      <c r="E90" t="inlineStr"/>
+      <c r="E90" t="n">
+        <v>2</v>
+      </c>
       <c r="F90" t="n">
         <v>0</v>
       </c>
@@ -2846,7 +2894,9 @@
       <c r="D91" s="2" t="n">
         <v>45544</v>
       </c>
-      <c r="E91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>99</v>
+      </c>
       <c r="F91" t="n">
         <v>0</v>
       </c>
@@ -3438,7 +3488,9 @@
       <c r="D113" s="2" t="n">
         <v>45554</v>
       </c>
-      <c r="E113" t="inlineStr"/>
+      <c r="E113" t="n">
+        <v>99</v>
+      </c>
       <c r="F113" t="n">
         <v>0</v>
       </c>
@@ -3490,7 +3542,9 @@
       <c r="D115" s="2" t="n">
         <v>45554</v>
       </c>
-      <c r="E115" t="inlineStr"/>
+      <c r="E115" t="n">
+        <v>99</v>
+      </c>
       <c r="F115" t="n">
         <v>0</v>
       </c>
@@ -3515,7 +3569,9 @@
       <c r="D116" s="2" t="n">
         <v>45554</v>
       </c>
-      <c r="E116" t="inlineStr"/>
+      <c r="E116" t="n">
+        <v>5</v>
+      </c>
       <c r="F116" t="n">
         <v>0</v>
       </c>
@@ -3891,7 +3947,9 @@
       <c r="D130" s="2" t="n">
         <v>45574</v>
       </c>
-      <c r="E130" t="inlineStr"/>
+      <c r="E130" t="n">
+        <v>99</v>
+      </c>
       <c r="F130" t="n">
         <v>0</v>
       </c>
@@ -4051,7 +4109,9 @@
       <c r="D136" s="2" t="n">
         <v>45574</v>
       </c>
-      <c r="E136" t="inlineStr"/>
+      <c r="E136" t="n">
+        <v>99</v>
+      </c>
       <c r="F136" t="n">
         <v>0</v>
       </c>
@@ -4076,7 +4136,9 @@
       <c r="D137" s="2" t="n">
         <v>45574</v>
       </c>
-      <c r="E137" t="inlineStr"/>
+      <c r="E137" t="n">
+        <v>99</v>
+      </c>
       <c r="F137" t="n">
         <v>0</v>
       </c>
@@ -4533,7 +4595,9 @@
       <c r="D154" s="2" t="n">
         <v>45615</v>
       </c>
-      <c r="E154" t="inlineStr"/>
+      <c r="E154" t="n">
+        <v>6</v>
+      </c>
       <c r="F154" t="n">
         <v>0</v>
       </c>
@@ -4909,7 +4973,9 @@
       <c r="D168" s="2" t="n">
         <v>45615</v>
       </c>
-      <c r="E168" t="inlineStr"/>
+      <c r="E168" t="n">
+        <v>2</v>
+      </c>
       <c r="F168" t="n">
         <v>0</v>
       </c>
@@ -5150,7 +5216,9 @@
       <c r="D177" s="2" t="n">
         <v>45623</v>
       </c>
-      <c r="E177" t="inlineStr"/>
+      <c r="E177" t="n">
+        <v>99</v>
+      </c>
       <c r="F177" t="n">
         <v>0</v>
       </c>
@@ -5229,7 +5297,9 @@
       <c r="D180" s="2" t="n">
         <v>45623</v>
       </c>
-      <c r="E180" t="inlineStr"/>
+      <c r="E180" t="n">
+        <v>99</v>
+      </c>
       <c r="F180" t="n">
         <v>0</v>
       </c>
@@ -5308,7 +5378,9 @@
       <c r="D183" s="2" t="n">
         <v>45625</v>
       </c>
-      <c r="E183" t="inlineStr"/>
+      <c r="E183" t="n">
+        <v>99</v>
+      </c>
       <c r="F183" t="n">
         <v>0</v>
       </c>
@@ -5333,7 +5405,9 @@
       <c r="D184" s="2" t="n">
         <v>45625</v>
       </c>
-      <c r="E184" t="inlineStr"/>
+      <c r="E184" t="n">
+        <v>6</v>
+      </c>
       <c r="F184" t="n">
         <v>0</v>
       </c>
@@ -5871,7 +5945,9 @@
       <c r="D204" s="2" t="n">
         <v>45636</v>
       </c>
-      <c r="E204" t="inlineStr"/>
+      <c r="E204" t="n">
+        <v>6</v>
+      </c>
       <c r="F204" t="n">
         <v>0</v>
       </c>
@@ -6004,7 +6080,9 @@
       <c r="D209" s="2" t="n">
         <v>45643</v>
       </c>
-      <c r="E209" t="inlineStr"/>
+      <c r="E209" t="n">
+        <v>2</v>
+      </c>
       <c r="F209" t="n">
         <v>0</v>
       </c>
@@ -6251,7 +6329,9 @@
       <c r="F218" t="n">
         <v>0</v>
       </c>
-      <c r="G218" t="inlineStr"/>
+      <c r="G218" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -6357,7 +6437,9 @@
       <c r="F222" t="n">
         <v>0</v>
       </c>
-      <c r="G222" t="inlineStr"/>
+      <c r="G222" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -6457,7 +6539,9 @@
       <c r="D226" s="2" t="n">
         <v>45643</v>
       </c>
-      <c r="E226" t="inlineStr"/>
+      <c r="E226" t="n">
+        <v>2</v>
+      </c>
       <c r="F226" t="n">
         <v>0</v>
       </c>
@@ -6482,7 +6566,9 @@
       <c r="D227" s="2" t="n">
         <v>45643</v>
       </c>
-      <c r="E227" t="inlineStr"/>
+      <c r="E227" t="n">
+        <v>2</v>
+      </c>
       <c r="F227" t="n">
         <v>0</v>
       </c>
@@ -6507,7 +6593,9 @@
       <c r="D228" s="2" t="n">
         <v>45643</v>
       </c>
-      <c r="E228" t="inlineStr"/>
+      <c r="E228" t="n">
+        <v>2</v>
+      </c>
       <c r="F228" t="n">
         <v>0</v>
       </c>
@@ -6586,7 +6674,9 @@
       <c r="D231" s="2" t="n">
         <v>45644</v>
       </c>
-      <c r="E231" t="inlineStr"/>
+      <c r="E231" t="n">
+        <v>99</v>
+      </c>
       <c r="F231" t="n">
         <v>0</v>
       </c>

</xml_diff>